<commit_message>
Versión completa y en línea por GitHub Pages (falta transferir el repositorio a Milena y entonces hacer la necesaria actualización de links en archivos index y hojas de vida cortas)
</commit_message>
<xml_diff>
--- a/data/award_en.xlsx
+++ b/data/award_en.xlsx
@@ -1,26 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub\JDL_CV\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub\Mile_CV\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB75F284-B307-4C4C-9AAB-03531748B379}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7966282C-2CB3-415A-BF5F-5236CC3481DE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4245" yWindow="3390" windowWidth="21600" windowHeight="11835" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1125" yWindow="1125" windowWidth="21600" windowHeight="11505" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="education" sheetId="1" r:id="rId1"/>
+    <sheet name="education" sheetId="2" r:id="rId1"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="33">
   <si>
     <t>what</t>
   </si>
@@ -37,42 +37,6 @@
     <t>why</t>
   </si>
   <si>
-    <t>Bogota, Colombia</t>
-  </si>
-  <si>
-    <t>Grindley Grants</t>
-  </si>
-  <si>
-    <t>Sep. 2014</t>
-  </si>
-  <si>
-    <t>Canterbury, UK</t>
-  </si>
-  <si>
-    <t>Francisco José de Caldas Scholarship for Doctoral Studies</t>
-  </si>
-  <si>
-    <t>Oct. 2010 - Oct. 2014</t>
-  </si>
-  <si>
-    <t>Annual Prize in Evolutionary Psychology</t>
-  </si>
-  <si>
-    <t>Oct. 2009</t>
-  </si>
-  <si>
-    <t>Liverpool, UK</t>
-  </si>
-  <si>
-    <t>University of Liverpool International Scholarship</t>
-  </si>
-  <si>
-    <t>Sep. 2008 - Sep. 2009</t>
-  </si>
-  <si>
-    <t>Scholarship-Loan Programme</t>
-  </si>
-  <si>
     <t>Dic. 2018</t>
   </si>
   <si>
@@ -82,74 +46,86 @@
     <t>VIII Excellence Awards</t>
   </si>
   <si>
-    <t>Dic. 2017</t>
-  </si>
-  <si>
     <t>Dic. 2019</t>
   </si>
   <si>
-    <t>VI Excellence Awards</t>
-  </si>
-  <si>
-    <t>Economics Prize</t>
-  </si>
-  <si>
-    <t>Sep. 2020</t>
-  </si>
-  <si>
-    <t>Cambridge, MA, USA.</t>
-  </si>
-  <si>
-    <t>Best overall performance in the MSc</t>
-  </si>
-  <si>
-    <t>IX Excellence Awards</t>
-  </si>
-  <si>
-    <t>Dic. 2022</t>
-  </si>
-  <si>
     <t>\href{https://www.unbosque.edu.co/}{Universidad El Bosque}</t>
   </si>
   <si>
-    <t>\href{https://improbable.com/ig/about-the-ig-nobel-prizes/}{Ig Nobel Prize}</t>
-  </si>
-  <si>
-    <t>\href{https://eps.ac.uk/}{Experimental Psychology Society}</t>
-  </si>
-  <si>
-    <t>\href{https://minciencias.gov.co/}{Minciencias}</t>
-  </si>
-  <si>
-    <t>\href{https://www.liverpool.ac.uk/life-sciences/}{School of Life Sciences} – University of Liverpool</t>
-  </si>
-  <si>
-    <t>\href{https://www.liverpool.ac.uk/}{University of Liverpool}</t>
-  </si>
-  <si>
-    <t>\href{https://www.colfuturo.org/}{Colfuturo}</t>
-  </si>
-  <si>
     <t>COP\$10.000.000</t>
   </si>
   <si>
-    <t>COP\$7.000.000</t>
-  </si>
-  <si>
     <t>COP\$5.000.000</t>
   </si>
   <si>
-    <t>For ‘trying to quantify the relationship between different countries’ national income inequality and the average amount of mouth-to-mouth kissing’  (\href{https://doi.org/10.1038/s41598-019-43267-7}{Watkins, et al., 2019})</t>
+    <t>X Excellence Awards</t>
+  </si>
+  <si>
+    <t>Dic. 2023</t>
+  </si>
+  <si>
+    <t>Bogotá, Colombia</t>
+  </si>
+  <si>
+    <t>COP\$2.500.000</t>
+  </si>
+  <si>
+    <t>Cum Laude Mention</t>
+  </si>
+  <si>
+    <t>Sep. 2018</t>
+  </si>
+  <si>
+    <t>\href{https://www.uv.es/}{Universidad de Valencia}</t>
+  </si>
+  <si>
+    <t>Valencia, España</t>
+  </si>
+  <si>
+    <t>PhD Thesis in Neurosciences</t>
+  </si>
+  <si>
+    <t>Nov.2011 - Nov.2012</t>
+  </si>
+  <si>
+    <t>\href{https://https://www.uv.es/uvcooperacion/es/becas-ayudas/ayudas-estudiantes-paises-cooperacion/becas-luisa-cardona.html/}{Universidad de Valencia}</t>
+  </si>
+  <si>
+    <t>Fee exemption for the Official Master's Degree</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Honorary Degree </t>
+  </si>
+  <si>
+    <t>Sep. 2007</t>
+  </si>
+  <si>
+    <t>\href{https://www.ucatolica.edu.co/}{Universidad Cátolica de Colombia}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Improved performance among undergraduate psychology students </t>
+  </si>
+  <si>
+    <t>Mention for excellence</t>
+  </si>
+  <si>
+    <t>Mar.2007</t>
+  </si>
+  <si>
+    <t>\href{https://https://www.ucatolica.edu.co/portal/Facultades/facultad-de-psicologia/}{Universidad Cátolica de Colombia}</t>
+  </si>
+  <si>
+    <t>Mention postgraduate scholarship for obtaining the highest score among the psychology students of the faculty and 3rd place nationally in the 2006 version of the Quality Examination for Higher Education in Colombia (ECAES).</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Luisa Cardona Scholarship </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="_-[$$-240A]\ * #,##0.00_-;\-[$$-240A]\ * #,##0.00_-;_-[$$-240A]\ * &quot;-&quot;??_-;_-@_-"/>
-  </numFmts>
-  <fonts count="19" x14ac:knownFonts="1">
+  <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -280,12 +256,6 @@
     <font>
       <sz val="11"/>
       <color theme="0"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -632,13 +602,10 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="42">
@@ -699,9 +666,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -739,7 +706,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -845,7 +812,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -987,225 +954,166 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E13"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{793BED96-2147-4B37-A1DD-7D67BAF289FC}">
+  <dimension ref="A1:E8"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="48" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="40.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="77.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="46.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="58" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="49" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+      <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>28</v>
+      <c r="A2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B2" t="s">
+        <v>13</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>36</v>
+        <v>9</v>
+      </c>
+      <c r="D2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>24</v>
+    <row r="3" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" t="s">
+        <v>8</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>25</v>
+        <v>9</v>
+      </c>
+      <c r="D3" t="s">
+        <v>14</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>39</v>
+        <v>11</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>21</v>
+      <c r="A4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" t="s">
+        <v>5</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>37</v>
+        <v>9</v>
+      </c>
+      <c r="D4" t="s">
+        <v>14</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
+      <c r="A5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B5" t="s">
+        <v>17</v>
+      </c>
+      <c r="C5" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B5" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="E5" s="2" t="s">
-        <v>38</v>
+      <c r="D5" t="s">
+        <v>19</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>20</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
+    <row r="6" spans="1:5" ht="75" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>32</v>
+      </c>
+      <c r="B6" t="s">
+        <v>21</v>
+      </c>
+      <c r="C6" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="B6" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="E6" s="2" t="s">
-        <v>38</v>
+      <c r="D6" t="s">
+        <v>19</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>7</v>
+      <c r="A7" t="s">
+        <v>24</v>
+      </c>
+      <c r="B7" t="s">
+        <v>25</v>
       </c>
       <c r="C7" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D7" t="s">
+        <v>14</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="75" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>28</v>
+      </c>
+      <c r="B8" t="s">
+        <v>29</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D8" t="s">
+        <v>14</v>
+      </c>
+      <c r="E8" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="D7" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E7" s="1"/>
-    </row>
-    <row r="8" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A8" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="E8" s="1"/>
-    </row>
-    <row r="9" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A9" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E9" s="1" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A10" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E10" s="1"/>
-    </row>
-    <row r="11" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A11" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="D11" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="E11" s="1"/>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" s="1"/>
-      <c r="B12" s="1"/>
-      <c r="C12" s="1"/>
-      <c r="D12" s="1"/>
-      <c r="E12" s="1"/>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" s="1"/>
-      <c r="B13" s="1"/>
-      <c r="C13" s="1"/>
-      <c r="D13" s="1"/>
-      <c r="E13" s="1"/>
     </row>
   </sheetData>
-  <phoneticPr fontId="18" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>